<commit_message>
Added new Text File_ ggui.txt
</commit_message>
<xml_diff>
--- a/HRMS_Candidate_WalkIn_01_01_2018.xlsx
+++ b/HRMS_Candidate_WalkIn_01_01_2018.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="61">
   <si>
     <r>
       <t xml:space="preserve">DEFECT TRACKING LOG  FOR  </t>
@@ -219,9 +219,6 @@
   </si>
   <si>
     <t>New</t>
-  </si>
-  <si>
-    <t>WalkIn_Nov_12</t>
   </si>
 </sst>
 </file>
@@ -706,7 +703,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1304,15 +1301,9 @@
       <c r="O17" s="3"/>
     </row>
     <row r="18" spans="1:15" ht="38.25" customHeight="1">
-      <c r="A18" s="6">
-        <v>12</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="8">
-        <v>211212</v>
-      </c>
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
       <c r="D18" s="7"/>
       <c r="E18" s="11"/>
       <c r="F18" s="9"/>

</xml_diff>